<commit_message>
Fix crash in maleClients screenPartner form
</commit_message>
<xml_diff>
--- a/app/config/tables/maleClients/forms/screenPartner/screenPartner.xlsx
+++ b/app/config/tables/maleClients/forms/screenPartner/screenPartner.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40880" windowHeight="26520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="221">
   <si>
     <t>type</t>
   </si>
@@ -673,13 +673,19 @@
     <t>is_willing</t>
   </si>
   <si>
-    <t>not(data('is_valid')) &amp;&amp; data('is_willing')</t>
-  </si>
-  <si>
-    <t>not(data('is_willing'))</t>
-  </si>
-  <si>
     <t>selected(data('client_consent'),'a0')</t>
+  </si>
+  <si>
+    <t>not(selected(data('agree_screening'),'a1'))</t>
+  </si>
+  <si>
+    <t>not(selected(data('curr_relationship'),'a1')) &amp;&amp; selected(data('agree_screening'),'a1')</t>
+  </si>
+  <si>
+    <t>model.isSessionVariable</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -756,8 +762,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="253">
+  <cellStyleXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1068,7 +1086,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="253">
+  <cellStyles count="265">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1195,6 +1213,12 @@
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1321,6 +1345,12 @@
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1655,13 +1685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1677,7 +1707,7 @@
     <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30">
+    <row r="1" spans="1:18" ht="45">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -1729,22 +1759,24 @@
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="C2" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="R1" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>140</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="15"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1752,625 +1784,699 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:17" s="3" customFormat="1">
-      <c r="C3" s="8" t="s">
+    <row r="3" spans="1:18">
+      <c r="C3" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="R3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="C4" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="R4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" s="3" customFormat="1">
+      <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:17" s="3" customFormat="1">
-      <c r="C4" s="8" t="s">
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:18" s="3" customFormat="1">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:17" s="3" customFormat="1" ht="45">
-      <c r="C5" s="8" t="s">
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:18" s="3" customFormat="1" ht="45">
+      <c r="C9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E9" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J5" s="17" t="b">
+      <c r="J9" s="17" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="135">
-      <c r="C6" s="8" t="s">
+    <row r="10" spans="1:18" ht="135">
+      <c r="C10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="11" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="C7" s="9" t="s">
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="C11" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="18" t="b">
+      <c r="J11" s="18" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="60">
-      <c r="C8" s="9" t="s">
+    <row r="12" spans="1:18" ht="60">
+      <c r="C12" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="L8" s="2" t="s">
+      <c r="J12" s="18"/>
+      <c r="L12" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="60">
-      <c r="C9" s="9" t="s">
+    <row r="13" spans="1:18" ht="60">
+      <c r="C13" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="L9" s="2" t="s">
+      <c r="J13" s="18"/>
+      <c r="L13" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="30">
-      <c r="A10" s="2" t="s">
+    <row r="14" spans="1:18" ht="45">
+      <c r="A14" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="1:17" ht="45">
-      <c r="C11" s="8" t="s">
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:18" ht="45">
+      <c r="C15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="11" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="5"/>
-      <c r="F12" s="3"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="5"/>
-      <c r="F13" s="3"/>
-      <c r="J13" s="18"/>
-    </row>
-    <row r="14" spans="1:17" ht="90">
-      <c r="C14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="30">
-      <c r="C15" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="G15" s="3"/>
       <c r="J15" s="18"/>
-      <c r="L15" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="5"/>
+      <c r="F16" s="3"/>
       <c r="J16" s="18"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="30">
       <c r="A17" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G17" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="5"/>
+      <c r="F17" s="3"/>
       <c r="J17" s="18"/>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:12" ht="90">
+      <c r="C18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30">
+      <c r="C19" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="J19" s="18"/>
+      <c r="L19" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="J18" s="18"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="C19" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J19" s="18"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="C20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="1:12" ht="30">
-      <c r="C21" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="J21" s="18"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="C22" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G22" s="3"/>
       <c r="J22" s="18"/>
     </row>
     <row r="23" spans="1:12">
       <c r="C23" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J23" s="18"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="C24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="2" t="s">
-        <v>174</v>
+      <c r="E24" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:12" ht="30">
       <c r="C25" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>63</v>
+        <v>154</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J25" s="18"/>
     </row>
     <row r="26" spans="1:12">
       <c r="C26" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="C27" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E27" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="1:12" ht="30">
+      <c r="C29" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="C30" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="1:12" ht="210">
-      <c r="C27" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="60">
-      <c r="C28" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="J28" s="18"/>
-      <c r="L28" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="C29" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="1:12" ht="30">
-      <c r="C30" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J30" s="17"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="J30" s="18"/>
+    </row>
+    <row r="31" spans="1:12" ht="210">
       <c r="C31" s="9" t="s">
         <v>170</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="60">
+      <c r="C32" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="J32" s="18"/>
+      <c r="L32" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="C33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" s="17"/>
+    </row>
+    <row r="34" spans="1:10" ht="30">
+      <c r="C34" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J34" s="17"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="C35" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E35" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J31" s="18"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="C32" s="9" t="s">
+      <c r="J35" s="18"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="C36" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J32" s="17"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="1:10" ht="45">
-      <c r="A34" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J34" s="17"/>
-    </row>
-    <row r="35" spans="1:10" ht="60">
-      <c r="C35" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:10" ht="75">
-      <c r="C36" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="J36" s="18"/>
+      <c r="J36" s="17"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="4"/>
-      <c r="J37" s="18"/>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="J37" s="17"/>
+    </row>
+    <row r="38" spans="1:10" ht="75">
       <c r="A38" s="2" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="4"/>
-      <c r="J38" s="18"/>
-    </row>
-    <row r="39" spans="1:10" ht="75">
-      <c r="C39" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="J38" s="17"/>
+    </row>
+    <row r="39" spans="1:10" ht="60">
+      <c r="C39" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="4"/>
       <c r="E39" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>127</v>
+        <v>213</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="J39" s="18"/>
     </row>
-    <row r="40" spans="1:10" s="3" customFormat="1" ht="60">
+    <row r="40" spans="1:10" ht="75">
       <c r="C40" s="10" t="s">
         <v>170</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="1:10" s="3" customFormat="1" ht="30">
-      <c r="A41" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>218</v>
+        <v>111</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J40" s="18"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="12"/>
-      <c r="J41" s="16"/>
-    </row>
-    <row r="42" spans="1:10" ht="45">
-      <c r="C42" s="9" t="s">
+      <c r="J41" s="18"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="4"/>
+      <c r="J42" s="18"/>
+    </row>
+    <row r="43" spans="1:10" ht="75">
+      <c r="C43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J43" s="18"/>
+    </row>
+    <row r="44" spans="1:10" s="3" customFormat="1" ht="60">
+      <c r="C44" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J44" s="16"/>
+    </row>
+    <row r="45" spans="1:10" s="3" customFormat="1" ht="30">
+      <c r="A45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="12"/>
+      <c r="J45" s="16"/>
+    </row>
+    <row r="46" spans="1:10" ht="45">
+      <c r="C46" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E46" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J42" s="17"/>
-    </row>
-    <row r="43" spans="1:10" ht="30">
-      <c r="A43" s="2" t="s">
+      <c r="J46" s="17"/>
+    </row>
+    <row r="47" spans="1:10" ht="30">
+      <c r="A47" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="J43" s="17"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="C44" s="9" t="s">
+      <c r="J47" s="17"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="C48" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J44" s="17"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="2" t="s">
+      <c r="J48" s="17"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="J45" s="17"/>
-    </row>
-    <row r="46" spans="1:10" ht="60">
-      <c r="C46" s="10" t="s">
+      <c r="J49" s="17"/>
+    </row>
+    <row r="50" spans="1:10" ht="60">
+      <c r="C50" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="11" t="s">
+      <c r="D50" s="4"/>
+      <c r="E50" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J46" s="18"/>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="2" t="s">
+      <c r="J50" s="18"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="4"/>
-      <c r="J47" s="18"/>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="2" t="s">
+      <c r="C51" s="10"/>
+      <c r="D51" s="4"/>
+      <c r="J51" s="18"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="4"/>
-      <c r="J48" s="18"/>
-    </row>
-    <row r="49" spans="3:10" ht="30">
-      <c r="C49" s="9" t="s">
+      <c r="C52" s="10"/>
+      <c r="D52" s="4"/>
+      <c r="J52" s="18"/>
+    </row>
+    <row r="53" spans="1:10" ht="30">
+      <c r="C53" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E53" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J49" s="18"/>
-    </row>
-    <row r="50" spans="3:10">
-      <c r="J50" s="18"/>
-    </row>
-    <row r="51" spans="3:10">
-      <c r="J51" s="18"/>
-    </row>
-    <row r="52" spans="3:10">
-      <c r="J52" s="18"/>
-    </row>
-    <row r="53" spans="3:10">
       <c r="J53" s="18"/>
     </row>
-    <row r="54" spans="3:10">
+    <row r="54" spans="1:10">
       <c r="J54" s="18"/>
     </row>
-    <row r="55" spans="3:10">
+    <row r="55" spans="1:10">
       <c r="J55" s="18"/>
     </row>
-    <row r="56" spans="3:10">
+    <row r="56" spans="1:10">
       <c r="J56" s="18"/>
     </row>
-    <row r="57" spans="3:10">
+    <row r="57" spans="1:10">
       <c r="J57" s="18"/>
     </row>
-    <row r="58" spans="3:10">
+    <row r="58" spans="1:10">
       <c r="J58" s="18"/>
     </row>
-    <row r="59" spans="3:10">
+    <row r="59" spans="1:10">
       <c r="J59" s="18"/>
     </row>
-    <row r="60" spans="3:10">
+    <row r="60" spans="1:10">
       <c r="J60" s="18"/>
     </row>
-    <row r="61" spans="3:10">
+    <row r="61" spans="1:10">
       <c r="J61" s="18"/>
     </row>
-    <row r="62" spans="3:10">
+    <row r="62" spans="1:10">
       <c r="J62" s="18"/>
     </row>
-    <row r="63" spans="3:10">
+    <row r="63" spans="1:10">
       <c r="J63" s="18"/>
     </row>
-    <row r="64" spans="3:10">
+    <row r="64" spans="1:10">
       <c r="J64" s="18"/>
     </row>
     <row r="65" spans="10:10">
@@ -2426,6 +2532,18 @@
     </row>
     <row r="82" spans="10:10">
       <c r="J82" s="18"/>
+    </row>
+    <row r="83" spans="10:10">
+      <c r="J83" s="18"/>
+    </row>
+    <row r="84" spans="10:10">
+      <c r="J84" s="18"/>
+    </row>
+    <row r="85" spans="10:10">
+      <c r="J85" s="18"/>
+    </row>
+    <row r="86" spans="10:10">
+      <c r="J86" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>